<commit_message>
Checks for positive pay
</commit_message>
<xml_diff>
--- a/data/raw/checks/peach tree checks.xlsx
+++ b/data/raw/checks/peach tree checks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HazTrain5\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE55C478-4AEF-4C99-AF3D-FB37A6DE62EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23060" windowHeight="14630"/>
+    <workbookView xWindow="-36020" yWindow="1990" windowWidth="35140" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Check Register'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="224">
   <si>
     <t>Check #</t>
   </si>
@@ -684,17 +696,32 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>12716</t>
+  </si>
+  <si>
+    <t>12717</t>
+  </si>
+  <si>
+    <t>12718</t>
+  </si>
+  <si>
+    <t>12719</t>
+  </si>
+  <si>
+    <t>12720</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00;* ??"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,6 +739,25 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -738,15 +784,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -755,9 +792,18 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -765,10 +811,10 @@
       <left/>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -776,38 +822,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,38 +1143,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E153"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="N147" sqref="N147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.6328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1126,7 +1182,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>45208</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1135,7 +1191,7 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="5">
         <v>-15000</v>
       </c>
     </row>
@@ -1143,7 +1199,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>45208</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1152,7 +1208,7 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>11000</v>
       </c>
     </row>
@@ -1160,7 +1216,7 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>45208</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1169,7 +1225,7 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>82791.91</v>
       </c>
     </row>
@@ -1177,7 +1233,7 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>45208</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1186,7 +1242,7 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>390</v>
       </c>
     </row>
@@ -1194,7 +1250,7 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>45208</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1203,7 +1259,7 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>14</v>
       </c>
     </row>
@@ -1211,7 +1267,7 @@
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>45208</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1220,7 +1276,7 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>926.71</v>
       </c>
     </row>
@@ -1228,7 +1284,7 @@
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>45208</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1237,7 +1293,7 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>60</v>
       </c>
     </row>
@@ -1245,7 +1301,7 @@
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>45208</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1254,7 +1310,7 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="5">
         <v>52.25</v>
       </c>
     </row>
@@ -1262,7 +1318,7 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>45208</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1271,7 +1327,7 @@
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="5">
         <v>2153.9899999999998</v>
       </c>
     </row>
@@ -1279,7 +1335,7 @@
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>45208</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1288,7 +1344,7 @@
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="5">
         <v>1916.07</v>
       </c>
     </row>
@@ -1296,7 +1352,7 @@
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>45208</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1305,7 +1361,7 @@
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="5">
         <v>595.66999999999996</v>
       </c>
     </row>
@@ -1313,7 +1369,7 @@
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>45208</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1322,7 +1378,7 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>217.56</v>
       </c>
     </row>
@@ -1330,7 +1386,7 @@
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>45208</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1339,7 +1395,7 @@
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="5">
         <v>4744.8100000000004</v>
       </c>
     </row>
@@ -1347,7 +1403,7 @@
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>45208</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1356,7 +1412,7 @@
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="5">
         <v>373.7</v>
       </c>
     </row>
@@ -1364,7 +1420,7 @@
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>45208</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1373,7 +1429,7 @@
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="5">
         <v>73.98</v>
       </c>
     </row>
@@ -1381,7 +1437,7 @@
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>45208</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1390,7 +1446,7 @@
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="5">
         <v>306.02</v>
       </c>
     </row>
@@ -1398,7 +1454,7 @@
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>45208</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1407,7 +1463,7 @@
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="5">
         <v>25.36</v>
       </c>
     </row>
@@ -1415,7 +1471,7 @@
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>45208</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1424,7 +1480,7 @@
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="5">
         <v>213.22</v>
       </c>
     </row>
@@ -1432,7 +1488,7 @@
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>45215</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1441,7 +1497,7 @@
       <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="5">
         <v>20747.71</v>
       </c>
     </row>
@@ -1449,7 +1505,7 @@
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <v>45215</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1458,7 +1514,7 @@
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="5">
         <v>552.66</v>
       </c>
     </row>
@@ -1466,7 +1522,7 @@
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <v>45215</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1475,7 +1531,7 @@
       <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="5">
         <v>528.08000000000004</v>
       </c>
     </row>
@@ -1483,7 +1539,7 @@
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <v>45215</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1492,7 +1548,7 @@
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="5">
         <v>17055.62</v>
       </c>
     </row>
@@ -1500,7 +1556,7 @@
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <v>45215</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1509,7 +1565,7 @@
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="5">
         <v>68633.84</v>
       </c>
     </row>
@@ -1517,7 +1573,7 @@
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>45215</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1526,7 +1582,7 @@
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="5">
         <v>454.35</v>
       </c>
     </row>
@@ -1534,7 +1590,7 @@
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>45215</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1543,7 +1599,7 @@
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="5">
         <v>660.1</v>
       </c>
     </row>
@@ -1551,7 +1607,7 @@
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <v>45215</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1560,7 +1616,7 @@
       <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="5">
         <v>171</v>
       </c>
     </row>
@@ -1568,7 +1624,7 @@
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>45215</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1577,7 +1633,7 @@
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="5">
         <v>1936.51</v>
       </c>
     </row>
@@ -1585,7 +1641,7 @@
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>45215</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1594,7 +1650,7 @@
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="5">
         <v>3578.71</v>
       </c>
     </row>
@@ -1602,7 +1658,7 @@
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="4">
         <v>45215</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1611,7 +1667,7 @@
       <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="5">
         <v>624.34</v>
       </c>
     </row>
@@ -1619,7 +1675,7 @@
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>45215</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1628,7 +1684,7 @@
       <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="5">
         <v>121.68</v>
       </c>
     </row>
@@ -1636,7 +1692,7 @@
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <v>45215</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1645,7 +1701,7 @@
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="5">
         <v>8272.84</v>
       </c>
     </row>
@@ -1653,7 +1709,7 @@
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="4">
         <v>45215</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1662,7 +1718,7 @@
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="5">
         <v>1489.04</v>
       </c>
     </row>
@@ -1670,7 +1726,7 @@
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="4">
         <v>45217</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1679,7 +1735,7 @@
       <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="5">
         <v>42395.8</v>
       </c>
     </row>
@@ -1687,7 +1743,7 @@
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>45217</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1696,7 +1752,7 @@
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="5">
         <v>850000</v>
       </c>
     </row>
@@ -1704,7 +1760,7 @@
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="4">
         <v>45223</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1713,7 +1769,7 @@
       <c r="D36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="5">
         <v>1802.28</v>
       </c>
     </row>
@@ -1721,7 +1777,7 @@
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="4">
         <v>45224</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1730,7 +1786,7 @@
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="5">
         <v>20607.53</v>
       </c>
     </row>
@@ -1738,7 +1794,7 @@
       <c r="A38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="4">
         <v>45225</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1747,7 +1803,7 @@
       <c r="D38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="5">
         <v>25329.81</v>
       </c>
     </row>
@@ -1755,7 +1811,7 @@
       <c r="A39" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="4">
         <v>45225</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1764,7 +1820,7 @@
       <c r="D39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="5">
         <v>1038.95</v>
       </c>
     </row>
@@ -1772,7 +1828,7 @@
       <c r="A40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="4">
         <v>45225</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -1781,7 +1837,7 @@
       <c r="D40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="5">
         <v>564.07000000000005</v>
       </c>
     </row>
@@ -1789,7 +1845,7 @@
       <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="4">
         <v>45225</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1798,7 +1854,7 @@
       <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="5">
         <v>920.44</v>
       </c>
     </row>
@@ -1806,7 +1862,7 @@
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="4">
         <v>45225</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1815,7 +1871,7 @@
       <c r="D42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="5">
         <v>104.98</v>
       </c>
     </row>
@@ -1823,7 +1879,7 @@
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="4">
         <v>45225</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1832,7 +1888,7 @@
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="5">
         <v>4637.6499999999996</v>
       </c>
     </row>
@@ -1840,7 +1896,7 @@
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="4">
         <v>45225</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -1849,7 +1905,7 @@
       <c r="D44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="5">
         <v>3226.05</v>
       </c>
     </row>
@@ -1857,7 +1913,7 @@
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="4">
         <v>45225</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1866,7 +1922,7 @@
       <c r="D45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="5">
         <v>12709.41</v>
       </c>
     </row>
@@ -1874,7 +1930,7 @@
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="4">
         <v>45225</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -1883,7 +1939,7 @@
       <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="5">
         <v>340.88</v>
       </c>
     </row>
@@ -1891,7 +1947,7 @@
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="4">
         <v>45225</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1900,7 +1956,7 @@
       <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="5">
         <v>2100</v>
       </c>
     </row>
@@ -1908,7 +1964,7 @@
       <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="4">
         <v>45229</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -1917,7 +1973,7 @@
       <c r="D48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="5">
         <v>11000</v>
       </c>
     </row>
@@ -1925,7 +1981,7 @@
       <c r="A49" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="4">
         <v>45229</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -1934,7 +1990,7 @@
       <c r="D49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E49" s="5">
         <v>264.04000000000002</v>
       </c>
     </row>
@@ -1942,7 +1998,7 @@
       <c r="A50" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="4">
         <v>45229</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -1951,7 +2007,7 @@
       <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="5">
         <v>1816.3</v>
       </c>
     </row>
@@ -1959,7 +2015,7 @@
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="4">
         <v>45229</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -1968,7 +2024,7 @@
       <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="5">
         <v>17604.080000000002</v>
       </c>
     </row>
@@ -1976,7 +2032,7 @@
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="4">
         <v>45229</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -1985,7 +2041,7 @@
       <c r="D52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="5">
         <v>10086.049999999999</v>
       </c>
     </row>
@@ -1993,7 +2049,7 @@
       <c r="A53" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="4">
         <v>45229</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -2002,7 +2058,7 @@
       <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="5">
         <v>31173.7</v>
       </c>
     </row>
@@ -2010,7 +2066,7 @@
       <c r="A54" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="4">
         <v>45229</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -2019,7 +2075,7 @@
       <c r="D54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="5">
         <v>3612.45</v>
       </c>
     </row>
@@ -2027,7 +2083,7 @@
       <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="4">
         <v>45229</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -2036,7 +2092,7 @@
       <c r="D55" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="5">
         <v>27.42</v>
       </c>
     </row>
@@ -2044,7 +2100,7 @@
       <c r="A56" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="4">
         <v>45229</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -2053,7 +2109,7 @@
       <c r="D56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="5">
         <v>152.63999999999999</v>
       </c>
     </row>
@@ -2061,7 +2117,7 @@
       <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="4">
         <v>45230</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -2070,7 +2126,7 @@
       <c r="D57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E57" s="5">
         <v>2862.28</v>
       </c>
     </row>
@@ -2078,7 +2134,7 @@
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="4">
         <v>45233</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2087,7 +2143,7 @@
       <c r="D58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="5">
         <v>104682.7</v>
       </c>
     </row>
@@ -2095,7 +2151,7 @@
       <c r="A59" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="4">
         <v>45233</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2104,7 +2160,7 @@
       <c r="D59" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="5">
         <v>348.75</v>
       </c>
     </row>
@@ -2112,7 +2168,7 @@
       <c r="A60" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="4">
         <v>45233</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -2121,7 +2177,7 @@
       <c r="D60" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E60" s="5">
         <v>270</v>
       </c>
     </row>
@@ -2129,7 +2185,7 @@
       <c r="A61" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="4">
         <v>45237</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -2138,7 +2194,7 @@
       <c r="D61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E61" s="5">
         <v>120</v>
       </c>
     </row>
@@ -2146,7 +2202,7 @@
       <c r="A62" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="4">
         <v>45237</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -2155,7 +2211,7 @@
       <c r="D62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="5">
         <v>10737.5</v>
       </c>
     </row>
@@ -2163,7 +2219,7 @@
       <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="4">
         <v>45237</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2172,7 +2228,7 @@
       <c r="D63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E63" s="5">
         <v>4610.13</v>
       </c>
     </row>
@@ -2180,7 +2236,7 @@
       <c r="A64" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="4">
         <v>45237</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2189,7 +2245,7 @@
       <c r="D64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E64" s="5">
         <v>2049.7199999999998</v>
       </c>
     </row>
@@ -2197,7 +2253,7 @@
       <c r="A65" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="4">
         <v>45237</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2206,7 +2262,7 @@
       <c r="D65" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="5">
         <v>313.01</v>
       </c>
     </row>
@@ -2214,7 +2270,7 @@
       <c r="A66" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="4">
         <v>45237</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2223,7 +2279,7 @@
       <c r="D66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E66" s="5">
         <v>241.5</v>
       </c>
     </row>
@@ -2231,7 +2287,7 @@
       <c r="A67" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="4">
         <v>45237</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2240,7 +2296,7 @@
       <c r="D67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="8">
+      <c r="E67" s="5">
         <v>78718.11</v>
       </c>
     </row>
@@ -2248,7 +2304,7 @@
       <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="4">
         <v>45237</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -2257,7 +2313,7 @@
       <c r="D68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E68" s="5">
         <v>95000</v>
       </c>
     </row>
@@ -2265,7 +2321,7 @@
       <c r="A69" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="4">
         <v>45237</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2274,7 +2330,7 @@
       <c r="D69" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69" s="5">
         <v>-95000</v>
       </c>
     </row>
@@ -2282,7 +2338,7 @@
       <c r="A70" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="4">
         <v>45238</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -2291,7 +2347,7 @@
       <c r="D70" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E70" s="5">
         <v>80000</v>
       </c>
     </row>
@@ -2299,7 +2355,7 @@
       <c r="A71" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="4">
         <v>45245</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2308,7 +2364,7 @@
       <c r="D71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="5">
         <v>2868.22</v>
       </c>
     </row>
@@ -2316,7 +2372,7 @@
       <c r="A72" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="4">
         <v>45245</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -2325,7 +2381,7 @@
       <c r="D72" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E72" s="8">
+      <c r="E72" s="5">
         <v>5262</v>
       </c>
     </row>
@@ -2333,7 +2389,7 @@
       <c r="A73" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="4">
         <v>45245</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -2342,7 +2398,7 @@
       <c r="D73" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="8">
+      <c r="E73" s="5">
         <v>-1038.95</v>
       </c>
     </row>
@@ -2350,7 +2406,7 @@
       <c r="A74" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="4">
         <v>45245</v>
       </c>
       <c r="C74" s="2" t="s">
@@ -2359,7 +2415,7 @@
       <c r="D74" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E74" s="5">
         <v>-564.07000000000005</v>
       </c>
     </row>
@@ -2367,7 +2423,7 @@
       <c r="A75" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="4">
         <v>45245</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -2376,7 +2432,7 @@
       <c r="D75" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="8">
+      <c r="E75" s="5">
         <v>-920.44</v>
       </c>
     </row>
@@ -2384,7 +2440,7 @@
       <c r="A76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="4">
         <v>45245</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -2393,7 +2449,7 @@
       <c r="D76" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E76" s="5">
         <v>-104.98</v>
       </c>
     </row>
@@ -2401,7 +2457,7 @@
       <c r="A77" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="4">
         <v>45245</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -2410,7 +2466,7 @@
       <c r="D77" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E77" s="5">
         <v>-4637.6499999999996</v>
       </c>
     </row>
@@ -2418,7 +2474,7 @@
       <c r="A78" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="4">
         <v>45245</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -2427,7 +2483,7 @@
       <c r="D78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E78" s="5">
         <v>-12709.41</v>
       </c>
     </row>
@@ -2435,7 +2491,7 @@
       <c r="A79" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="4">
         <v>45245</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -2444,7 +2500,7 @@
       <c r="D79" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E79" s="5">
         <v>-2100</v>
       </c>
     </row>
@@ -2452,7 +2508,7 @@
       <c r="A80" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="4">
         <v>45245</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -2461,7 +2517,7 @@
       <c r="D80" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E80" s="5">
         <v>2100</v>
       </c>
     </row>
@@ -2469,7 +2525,7 @@
       <c r="A81" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="4">
         <v>45245</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -2478,7 +2534,7 @@
       <c r="D81" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E81" s="5">
         <v>1038.95</v>
       </c>
     </row>
@@ -2486,7 +2542,7 @@
       <c r="A82" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="4">
         <v>45245</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -2495,7 +2551,7 @@
       <c r="D82" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82" s="5">
         <v>564.07000000000005</v>
       </c>
     </row>
@@ -2503,7 +2559,7 @@
       <c r="A83" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="4">
         <v>45245</v>
       </c>
       <c r="C83" s="2" t="s">
@@ -2512,7 +2568,7 @@
       <c r="D83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E83" s="5">
         <v>1417.05</v>
       </c>
     </row>
@@ -2520,7 +2576,7 @@
       <c r="A84" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="4">
         <v>45245</v>
       </c>
       <c r="C84" s="2" t="s">
@@ -2529,7 +2585,7 @@
       <c r="D84" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E84" s="5">
         <v>104.98</v>
       </c>
     </row>
@@ -2537,7 +2593,7 @@
       <c r="A85" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="4">
         <v>45245</v>
       </c>
       <c r="C85" s="2" t="s">
@@ -2546,7 +2602,7 @@
       <c r="D85" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E85" s="5">
         <v>4637.6499999999996</v>
       </c>
     </row>
@@ -2554,7 +2610,7 @@
       <c r="A86" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="4">
         <v>45245</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -2563,7 +2619,7 @@
       <c r="D86" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86" s="5">
         <v>12709.41</v>
       </c>
     </row>
@@ -2571,7 +2627,7 @@
       <c r="A87" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="4">
         <v>45251</v>
       </c>
       <c r="C87" s="2" t="s">
@@ -2580,7 +2636,7 @@
       <c r="D87" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E87" s="8">
+      <c r="E87" s="5">
         <v>552.66</v>
       </c>
     </row>
@@ -2588,7 +2644,7 @@
       <c r="A88" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="4">
         <v>45251</v>
       </c>
       <c r="C88" s="2" t="s">
@@ -2597,7 +2653,7 @@
       <c r="D88" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E88" s="8">
+      <c r="E88" s="5">
         <v>1816.3</v>
       </c>
     </row>
@@ -2605,7 +2661,7 @@
       <c r="A89" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="4">
         <v>45251</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -2614,7 +2670,7 @@
       <c r="D89" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E89" s="5">
         <v>382.28</v>
       </c>
     </row>
@@ -2622,7 +2678,7 @@
       <c r="A90" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="4">
         <v>45251</v>
       </c>
       <c r="C90" s="2" t="s">
@@ -2631,7 +2687,7 @@
       <c r="D90" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E90" s="5">
         <v>454.35</v>
       </c>
     </row>
@@ -2639,7 +2695,7 @@
       <c r="A91" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="4">
         <v>45251</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -2648,7 +2704,7 @@
       <c r="D91" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="8">
+      <c r="E91" s="5">
         <v>163.24</v>
       </c>
     </row>
@@ -2656,7 +2712,7 @@
       <c r="A92" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="4">
         <v>45251</v>
       </c>
       <c r="C92" s="2" t="s">
@@ -2665,7 +2721,7 @@
       <c r="D92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="8">
+      <c r="E92" s="5">
         <v>855.27</v>
       </c>
     </row>
@@ -2673,7 +2729,7 @@
       <c r="A93" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="4">
         <v>45251</v>
       </c>
       <c r="C93" s="2" t="s">
@@ -2682,7 +2738,7 @@
       <c r="D93" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="8">
+      <c r="E93" s="5">
         <v>171</v>
       </c>
     </row>
@@ -2690,7 +2746,7 @@
       <c r="A94" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="4">
         <v>45251</v>
       </c>
       <c r="C94" s="2" t="s">
@@ -2699,7 +2755,7 @@
       <c r="D94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="8">
+      <c r="E94" s="5">
         <v>1870.27</v>
       </c>
     </row>
@@ -2707,7 +2763,7 @@
       <c r="A95" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="4">
         <v>45251</v>
       </c>
       <c r="C95" s="2" t="s">
@@ -2716,7 +2772,7 @@
       <c r="D95" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E95" s="8">
+      <c r="E95" s="5">
         <v>624.34</v>
       </c>
     </row>
@@ -2724,7 +2780,7 @@
       <c r="A96" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="4">
         <v>45251</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -2733,7 +2789,7 @@
       <c r="D96" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="8">
+      <c r="E96" s="5">
         <v>438.7</v>
       </c>
     </row>
@@ -2741,7 +2797,7 @@
       <c r="A97" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="4">
         <v>45251</v>
       </c>
       <c r="C97" s="2" t="s">
@@ -2750,7 +2806,7 @@
       <c r="D97" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="8">
+      <c r="E97" s="5">
         <v>329.8</v>
       </c>
     </row>
@@ -2758,7 +2814,7 @@
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="4">
         <v>45251</v>
       </c>
       <c r="C98" s="2" t="s">
@@ -2767,7 +2823,7 @@
       <c r="D98" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E98" s="5">
         <v>382.28</v>
       </c>
     </row>
@@ -2775,7 +2831,7 @@
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="4">
         <v>45257</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -2784,7 +2840,7 @@
       <c r="D99" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="8">
+      <c r="E99" s="5">
         <v>1824.54</v>
       </c>
     </row>
@@ -2792,7 +2848,7 @@
       <c r="A100" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="4">
         <v>45257</v>
       </c>
       <c r="C100" s="2" t="s">
@@ -2801,7 +2857,7 @@
       <c r="D100" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="8">
+      <c r="E100" s="5">
         <v>3372.74</v>
       </c>
     </row>
@@ -2809,7 +2865,7 @@
       <c r="A101" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="4">
         <v>45272</v>
       </c>
       <c r="C101" s="2" t="s">
@@ -2818,7 +2874,7 @@
       <c r="D101" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="8">
+      <c r="E101" s="5">
         <v>5500</v>
       </c>
     </row>
@@ -2826,7 +2882,7 @@
       <c r="A102" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="4">
         <v>45272</v>
       </c>
       <c r="C102" s="2" t="s">
@@ -2835,7 +2891,7 @@
       <c r="D102" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="8">
+      <c r="E102" s="5">
         <v>528.08000000000004</v>
       </c>
     </row>
@@ -2843,7 +2899,7 @@
       <c r="A103" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="4">
         <v>45272</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -2852,7 +2908,7 @@
       <c r="D103" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E103" s="8">
+      <c r="E103" s="5">
         <v>1825</v>
       </c>
     </row>
@@ -2860,7 +2916,7 @@
       <c r="A104" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="4">
         <v>45272</v>
       </c>
       <c r="C104" s="2" t="s">
@@ -2869,7 +2925,7 @@
       <c r="D104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="8">
+      <c r="E104" s="5">
         <v>11000</v>
       </c>
     </row>
@@ -2877,7 +2933,7 @@
       <c r="A105" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="4">
         <v>45272</v>
       </c>
       <c r="C105" s="2" t="s">
@@ -2886,7 +2942,7 @@
       <c r="D105" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E105" s="8">
+      <c r="E105" s="5">
         <v>771.38</v>
       </c>
     </row>
@@ -2894,7 +2950,7 @@
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="4">
         <v>45272</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -2903,7 +2959,7 @@
       <c r="D106" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E106" s="8">
+      <c r="E106" s="5">
         <v>255.26</v>
       </c>
     </row>
@@ -2911,7 +2967,7 @@
       <c r="A107" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="4">
         <v>45272</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -2920,7 +2976,7 @@
       <c r="D107" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E107" s="8">
+      <c r="E107" s="5">
         <v>91.86</v>
       </c>
     </row>
@@ -2928,7 +2984,7 @@
       <c r="A108" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="4">
         <v>45272</v>
       </c>
       <c r="C108" s="2" t="s">
@@ -2937,7 +2993,7 @@
       <c r="D108" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E108" s="8">
+      <c r="E108" s="5">
         <v>7936.75</v>
       </c>
     </row>
@@ -2945,7 +3001,7 @@
       <c r="A109" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B109" s="4">
         <v>45272</v>
       </c>
       <c r="C109" s="2" t="s">
@@ -2954,7 +3010,7 @@
       <c r="D109" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E109" s="8">
+      <c r="E109" s="5">
         <v>454.35</v>
       </c>
     </row>
@@ -2962,7 +3018,7 @@
       <c r="A110" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="4">
         <v>45272</v>
       </c>
       <c r="C110" s="2" t="s">
@@ -2971,7 +3027,7 @@
       <c r="D110" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E110" s="8">
+      <c r="E110" s="5">
         <v>12250</v>
       </c>
     </row>
@@ -2979,7 +3035,7 @@
       <c r="A111" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="4">
         <v>45272</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -2988,7 +3044,7 @@
       <c r="D111" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E111" s="8">
+      <c r="E111" s="5">
         <v>1920</v>
       </c>
     </row>
@@ -2996,7 +3052,7 @@
       <c r="A112" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="4">
         <v>45272</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -3005,7 +3061,7 @@
       <c r="D112" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E112" s="8">
+      <c r="E112" s="5">
         <v>1742.27</v>
       </c>
     </row>
@@ -3013,7 +3069,7 @@
       <c r="A113" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B113" s="4">
         <v>45272</v>
       </c>
       <c r="C113" s="2" t="s">
@@ -3022,7 +3078,7 @@
       <c r="D113" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E113" s="8">
+      <c r="E113" s="5">
         <v>171</v>
       </c>
     </row>
@@ -3030,7 +3086,7 @@
       <c r="A114" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="4">
         <v>45272</v>
       </c>
       <c r="C114" s="2" t="s">
@@ -3039,7 +3095,7 @@
       <c r="D114" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E114" s="8">
+      <c r="E114" s="5">
         <v>2930.94</v>
       </c>
     </row>
@@ -3047,7 +3103,7 @@
       <c r="A115" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="4">
         <v>45272</v>
       </c>
       <c r="C115" s="2" t="s">
@@ -3056,7 +3112,7 @@
       <c r="D115" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E115" s="8">
+      <c r="E115" s="5">
         <v>326.52</v>
       </c>
     </row>
@@ -3064,7 +3120,7 @@
       <c r="A116" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="4">
         <v>45272</v>
       </c>
       <c r="C116" s="2" t="s">
@@ -3073,7 +3129,7 @@
       <c r="D116" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E116" s="8">
+      <c r="E116" s="5">
         <v>531</v>
       </c>
     </row>
@@ -3081,7 +3137,7 @@
       <c r="A117" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B117" s="4">
         <v>45272</v>
       </c>
       <c r="C117" s="2" t="s">
@@ -3090,7 +3146,7 @@
       <c r="D117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E117" s="8">
+      <c r="E117" s="5">
         <v>18635</v>
       </c>
     </row>
@@ -3098,7 +3154,7 @@
       <c r="A118" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="4">
         <v>45272</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -3107,7 +3163,7 @@
       <c r="D118" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E118" s="8">
+      <c r="E118" s="5">
         <v>319.99</v>
       </c>
     </row>
@@ -3115,7 +3171,7 @@
       <c r="A119" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="4">
         <v>45272</v>
       </c>
       <c r="C119" s="2" t="s">
@@ -3124,7 +3180,7 @@
       <c r="D119" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="8">
+      <c r="E119" s="5">
         <v>583.27</v>
       </c>
     </row>
@@ -3132,7 +3188,7 @@
       <c r="A120" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="4">
         <v>45272</v>
       </c>
       <c r="C120" s="2" t="s">
@@ -3141,7 +3197,7 @@
       <c r="D120" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="8">
+      <c r="E120" s="5">
         <v>195</v>
       </c>
     </row>
@@ -3149,7 +3205,7 @@
       <c r="A121" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B121" s="4">
         <v>45272</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -3158,7 +3214,7 @@
       <c r="D121" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E121" s="8">
+      <c r="E121" s="5">
         <v>100.24</v>
       </c>
     </row>
@@ -3166,7 +3222,7 @@
       <c r="A122" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="4">
         <v>45272</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -3175,7 +3231,7 @@
       <c r="D122" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E122" s="8">
+      <c r="E122" s="5">
         <v>288</v>
       </c>
     </row>
@@ -3183,7 +3239,7 @@
       <c r="A123" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B123" s="6">
+      <c r="B123" s="4">
         <v>45272</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -3192,7 +3248,7 @@
       <c r="D123" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E123" s="8">
+      <c r="E123" s="5">
         <v>552.66</v>
       </c>
     </row>
@@ -3200,7 +3256,7 @@
       <c r="A124" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="4">
         <v>45274</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -3209,7 +3265,7 @@
       <c r="D124" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E124" s="8">
+      <c r="E124" s="5">
         <v>112</v>
       </c>
     </row>
@@ -3217,7 +3273,7 @@
       <c r="A125" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B125" s="6">
+      <c r="B125" s="4">
         <v>45275</v>
       </c>
       <c r="C125" s="2" t="s">
@@ -3226,7 +3282,7 @@
       <c r="D125" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E125" s="8">
+      <c r="E125" s="5">
         <v>84466.37</v>
       </c>
     </row>
@@ -3234,7 +3290,7 @@
       <c r="A126" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B126" s="4">
         <v>45275</v>
       </c>
       <c r="C126" s="2" t="s">
@@ -3243,7 +3299,7 @@
       <c r="D126" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E126" s="8">
+      <c r="E126" s="5">
         <v>31594.9</v>
       </c>
     </row>
@@ -3251,7 +3307,7 @@
       <c r="A127" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B127" s="4">
         <v>45275</v>
       </c>
       <c r="C127" s="2" t="s">
@@ -3265,7 +3321,7 @@
       <c r="A128" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="4">
         <v>45275</v>
       </c>
       <c r="C128" s="2" t="s">
@@ -3279,7 +3335,7 @@
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B129" s="4">
         <v>45275</v>
       </c>
       <c r="C129" s="2" t="s">
@@ -3288,7 +3344,7 @@
       <c r="D129" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E129" s="8">
+      <c r="E129" s="5">
         <v>660.1</v>
       </c>
     </row>
@@ -3296,7 +3352,7 @@
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="4">
         <v>45275</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -3305,7 +3361,7 @@
       <c r="D130" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E130" s="8">
+      <c r="E130" s="5">
         <v>17604.080000000002</v>
       </c>
     </row>
@@ -3313,7 +3369,7 @@
       <c r="A131" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B131" s="4">
         <v>45275</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -3322,7 +3378,7 @@
       <c r="D131" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E131" s="8">
+      <c r="E131" s="5">
         <v>356.05</v>
       </c>
     </row>
@@ -3330,7 +3386,7 @@
       <c r="A132" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="4">
         <v>45275</v>
       </c>
       <c r="C132" s="2" t="s">
@@ -3339,7 +3395,7 @@
       <c r="D132" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E132" s="8">
+      <c r="E132" s="5">
         <v>721.67</v>
       </c>
     </row>
@@ -3347,7 +3403,7 @@
       <c r="A133" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B133" s="4">
         <v>45275</v>
       </c>
       <c r="C133" s="2" t="s">
@@ -3356,7 +3412,7 @@
       <c r="D133" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E133" s="8">
+      <c r="E133" s="5">
         <v>26207.99</v>
       </c>
     </row>
@@ -3364,7 +3420,7 @@
       <c r="A134" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="4">
         <v>45275</v>
       </c>
       <c r="C134" s="2" t="s">
@@ -3373,7 +3429,7 @@
       <c r="D134" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E134" s="8">
+      <c r="E134" s="5">
         <v>25992.240000000002</v>
       </c>
     </row>
@@ -3381,7 +3437,7 @@
       <c r="A135" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B135" s="4">
         <v>45275</v>
       </c>
       <c r="C135" s="2" t="s">
@@ -3390,7 +3446,7 @@
       <c r="D135" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E135" s="8">
+      <c r="E135" s="5">
         <v>437.13</v>
       </c>
     </row>
@@ -3398,7 +3454,7 @@
       <c r="A136" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="4">
         <v>45275</v>
       </c>
       <c r="C136" s="2" t="s">
@@ -3407,7 +3463,7 @@
       <c r="D136" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E136" s="8">
+      <c r="E136" s="5">
         <v>819.24</v>
       </c>
     </row>
@@ -3415,7 +3471,7 @@
       <c r="A137" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B137" s="4">
         <v>45275</v>
       </c>
       <c r="C137" s="2" t="s">
@@ -3424,7 +3480,7 @@
       <c r="D137" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E137" s="8">
+      <c r="E137" s="5">
         <v>552.08000000000004</v>
       </c>
     </row>
@@ -3432,7 +3488,7 @@
       <c r="A138" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="4">
         <v>45275</v>
       </c>
       <c r="C138" s="2" t="s">
@@ -3441,7 +3497,7 @@
       <c r="D138" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E138" s="8">
+      <c r="E138" s="5">
         <v>3.71</v>
       </c>
     </row>
@@ -3449,7 +3505,7 @@
       <c r="A139" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B139" s="4">
         <v>45275</v>
       </c>
       <c r="C139" s="2" t="s">
@@ -3458,7 +3514,7 @@
       <c r="D139" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E139" s="8">
+      <c r="E139" s="5">
         <v>2210.7800000000002</v>
       </c>
     </row>
@@ -3466,7 +3522,7 @@
       <c r="A140" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="4">
         <v>45275</v>
       </c>
       <c r="C140" s="2" t="s">
@@ -3475,7 +3531,7 @@
       <c r="D140" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E140" s="8">
+      <c r="E140" s="5">
         <v>1435.63</v>
       </c>
     </row>
@@ -3483,7 +3539,7 @@
       <c r="A141" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B141" s="4">
         <v>45275</v>
       </c>
       <c r="C141" s="2" t="s">
@@ -3492,7 +3548,7 @@
       <c r="D141" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E141" s="8">
+      <c r="E141" s="5">
         <v>624.34</v>
       </c>
     </row>
@@ -3500,7 +3556,7 @@
       <c r="A142" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="4">
         <v>45275</v>
       </c>
       <c r="C142" s="2" t="s">
@@ -3509,7 +3565,7 @@
       <c r="D142" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E142" s="8">
+      <c r="E142" s="5">
         <v>128.57</v>
       </c>
     </row>
@@ -3517,7 +3573,7 @@
       <c r="A143" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B143" s="4">
         <v>45275</v>
       </c>
       <c r="C143" s="2" t="s">
@@ -3526,7 +3582,7 @@
       <c r="D143" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E143" s="8">
+      <c r="E143" s="5">
         <v>8824.0499999999993</v>
       </c>
     </row>
@@ -3534,7 +3590,7 @@
       <c r="A144" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="4">
         <v>45275</v>
       </c>
       <c r="C144" s="2" t="s">
@@ -3543,7 +3599,7 @@
       <c r="D144" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E144" s="8">
+      <c r="E144" s="5">
         <v>20835.36</v>
       </c>
     </row>
@@ -3551,7 +3607,7 @@
       <c r="A145" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B145" s="4">
         <v>45275</v>
       </c>
       <c r="C145" s="2" t="s">
@@ -3560,7 +3616,7 @@
       <c r="D145" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E145" s="8">
+      <c r="E145" s="5">
         <v>451.02</v>
       </c>
     </row>
@@ -3568,7 +3624,7 @@
       <c r="A146" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="4">
         <v>45275</v>
       </c>
       <c r="C146" s="2" t="s">
@@ -3577,7 +3633,7 @@
       <c r="D146" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E146" s="8">
+      <c r="E146" s="5">
         <v>-31594.9</v>
       </c>
     </row>
@@ -3585,7 +3641,7 @@
       <c r="A147" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B147" s="6">
+      <c r="B147" s="4">
         <v>45282</v>
       </c>
       <c r="C147" s="2" t="s">
@@ -3594,7 +3650,7 @@
       <c r="D147" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E147" s="8">
+      <c r="E147" s="5">
         <v>16751.580000000002</v>
       </c>
     </row>
@@ -3602,7 +3658,7 @@
       <c r="A148" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="4">
         <v>45282</v>
       </c>
       <c r="C148" s="2" t="s">
@@ -3611,7 +3667,7 @@
       <c r="D148" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E148" s="8">
+      <c r="E148" s="5">
         <v>14843.32</v>
       </c>
     </row>
@@ -3619,7 +3675,7 @@
       <c r="A149" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B149" s="6">
+      <c r="B149" s="4">
         <v>45282</v>
       </c>
       <c r="C149" s="2" t="s">
@@ -3633,7 +3689,7 @@
       <c r="A150" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="4">
         <v>45282</v>
       </c>
       <c r="C150" s="2" t="s">
@@ -3643,31 +3699,154 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="E151" s="12"/>
-    </row>
-    <row r="152" spans="1:5" s="4" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="3" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B151" s="11">
+        <v>45282</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D151" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E151" s="12">
+        <v>16751.580000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B152" s="11">
+        <v>45282</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E152" s="12">
+        <v>14843.32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B153" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E153" s="12">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B154" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C154" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D154" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" s="12">
+        <v>26208.49</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B155" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D155" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="12">
+        <v>518.53</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B156" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D156" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B157" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C157" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D157" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="12">
+        <v>831.49</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="13"/>
+    </row>
+    <row r="159" spans="1:5" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B152" s="5"/>
-      <c r="C152" s="3" t="s">
+      <c r="B159" s="15"/>
+      <c r="C159" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D159" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="E152" s="7">
-        <f>SUBTOTAL(9, E2:E151)</f>
-        <v>1856960.4400000004</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="13"/>
-      <c r="B153" s="13"/>
-      <c r="C153" s="13"/>
-      <c r="D153" s="13"/>
-      <c r="E153" s="14"/>
+      <c r="E159" s="16">
+        <f>SUBTOTAL(9, E151:E158)</f>
+        <v>70483.41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A160" s="17"/>
+      <c r="B160" s="17"/>
+      <c r="C160" s="17"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="1.25" bottom="0.65277777777777779" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
checks from peach tree
</commit_message>
<xml_diff>
--- a/data/raw/checks/peach tree checks.xlsx
+++ b/data/raw/checks/peach tree checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711A03AA-817B-4FDA-8E11-340930A43747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D31AFA7-CD4A-4CCD-9486-18519F38D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37710" yWindow="2340" windowWidth="34570" windowHeight="16790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29260" yWindow="290" windowWidth="27930" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -870,7 +870,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,6 +880,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -984,13 +1008,40 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1276,15 +1327,15 @@
   <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G178" sqref="G178"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K182" sqref="K182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
@@ -1937,87 +1988,87 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="25">
         <v>45225</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="5">
+      <c r="D39" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="26">
         <v>1038.95</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="25">
         <v>45225</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="D40" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="26">
         <v>564.07000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="25">
         <v>45225</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="5">
+      <c r="D41" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="26">
         <v>920.44</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="25">
         <v>45225</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="D42" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="26">
         <v>104.98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="25">
         <v>45225</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="5">
+      <c r="D43" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="26">
         <v>4637.6499999999996</v>
       </c>
     </row>
@@ -2039,19 +2090,19 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="25">
         <v>45225</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="D45" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="26">
         <v>12709.41</v>
       </c>
     </row>
@@ -2073,19 +2124,19 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="25">
         <v>45225</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="5">
+      <c r="D47" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="26">
         <v>2100</v>
       </c>
     </row>
@@ -2515,240 +2566,240 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="22">
         <v>45245</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="5">
+      <c r="D73" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="23">
         <v>-1038.95</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="22">
         <v>45245</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="5">
+      <c r="D74" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="23">
         <v>-564.07000000000005</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="22">
         <v>45245</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" s="5">
+      <c r="D75" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="23">
         <v>-920.44</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="22">
         <v>45245</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="5">
+      <c r="D76" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="23">
         <v>-104.98</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="22">
         <v>45245</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" s="5">
+      <c r="D77" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="23">
         <v>-4637.6499999999996</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78" s="22">
         <v>45245</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" s="5">
+      <c r="D78" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="23">
         <v>-12709.41</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79" s="22">
         <v>45245</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" s="5">
+      <c r="D79" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="23">
         <v>-2100</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80" s="28">
         <v>45245</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" s="5">
+      <c r="D80" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="29">
         <v>2100</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81" s="28">
         <v>45245</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="5">
+      <c r="D81" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="29">
         <v>1038.95</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82" s="28">
         <v>45245</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" s="5">
+      <c r="D82" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="29">
         <v>564.07000000000005</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83" s="28">
         <v>45245</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="5">
+      <c r="D83" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="29">
         <v>1417.05</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B84" s="28">
         <v>45245</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="5">
+      <c r="D84" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="29">
         <v>104.98</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B85" s="4">
+      <c r="B85" s="28">
         <v>45245</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="5">
+      <c r="D85" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="29">
         <v>4637.6499999999996</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B86" s="28">
         <v>45245</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="5">
+      <c r="D86" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="29">
         <v>12709.41</v>
       </c>
     </row>
@@ -3297,19 +3348,19 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="B119" s="4">
+      <c r="B119" s="31">
         <v>45272</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E119" s="5">
+      <c r="D119" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="32">
         <v>583.27</v>
       </c>
     </row>
@@ -4152,374 +4203,374 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="21" t="s">
+      <c r="A170" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B170" s="22">
+      <c r="B170" s="11">
         <v>45316</v>
       </c>
-      <c r="C170" s="21" t="s">
+      <c r="C170" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D170" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E170" s="23">
+      <c r="D170" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E170" s="12">
         <v>11000</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="21" t="s">
+      <c r="A171" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="B171" s="22">
+      <c r="B171" s="11">
         <v>45316</v>
       </c>
-      <c r="C171" s="21" t="s">
+      <c r="C171" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D171" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E171" s="23">
+      <c r="D171" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E171" s="12">
         <v>264.04000000000002</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="21" t="s">
+      <c r="A172" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B172" s="22">
+      <c r="B172" s="11">
         <v>45316</v>
       </c>
-      <c r="C172" s="21" t="s">
+      <c r="C172" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D172" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E172" s="23">
+      <c r="D172" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="12">
         <v>11700</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="21" t="s">
+      <c r="A173" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B173" s="22">
+      <c r="B173" s="11">
         <v>45316</v>
       </c>
-      <c r="C173" s="21" t="s">
+      <c r="C173" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D173" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E173" s="23">
+      <c r="D173" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" s="12">
         <v>501.75</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="21" t="s">
+      <c r="A174" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B174" s="22">
+      <c r="B174" s="11">
         <v>45316</v>
       </c>
-      <c r="C174" s="21" t="s">
+      <c r="C174" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D174" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E174" s="23">
+      <c r="D174" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E174" s="12">
         <v>41.25</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="21" t="s">
+      <c r="A175" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B175" s="22">
+      <c r="B175" s="11">
         <v>45316</v>
       </c>
-      <c r="C175" s="21" t="s">
+      <c r="C175" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D175" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E175" s="23">
+      <c r="D175" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E175" s="12">
         <v>17500</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="21" t="s">
+      <c r="A176" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="B176" s="22">
+      <c r="B176" s="11">
         <v>45316</v>
       </c>
-      <c r="C176" s="21" t="s">
+      <c r="C176" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D176" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E176" s="23">
+      <c r="D176" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" s="12">
         <v>2212.8200000000002</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="21" t="s">
+      <c r="A177" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B177" s="22">
+      <c r="B177" s="11">
         <v>45316</v>
       </c>
-      <c r="C177" s="21" t="s">
+      <c r="C177" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D177" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E177" s="23">
+      <c r="D177" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E177" s="12">
         <v>2617.4499999999998</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="21" t="s">
+      <c r="A178" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="B178" s="22">
+      <c r="B178" s="11">
         <v>45316</v>
       </c>
-      <c r="C178" s="21" t="s">
+      <c r="C178" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D178" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E178" s="23"/>
+      <c r="D178" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E178" s="12"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="21" t="s">
+      <c r="A179" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B179" s="22">
+      <c r="B179" s="11">
         <v>45316</v>
       </c>
-      <c r="C179" s="21" t="s">
+      <c r="C179" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D179" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E179" s="23">
+      <c r="D179" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E179" s="12">
         <v>171</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="21" t="s">
+      <c r="A180" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B180" s="22">
+      <c r="B180" s="11">
         <v>45316</v>
       </c>
-      <c r="C180" s="21" t="s">
+      <c r="C180" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D180" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E180" s="23">
+      <c r="D180" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" s="12">
         <v>199.16</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="21" t="s">
+      <c r="A181" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B181" s="22">
+      <c r="B181" s="11">
         <v>45316</v>
       </c>
-      <c r="C181" s="21" t="s">
+      <c r="C181" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="D181" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E181" s="23">
+      <c r="D181" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" s="12">
         <v>117.7</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="21" t="s">
+      <c r="A182" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B182" s="22">
+      <c r="B182" s="11">
         <v>45316</v>
       </c>
-      <c r="C182" s="21" t="s">
+      <c r="C182" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D182" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E182" s="23">
+      <c r="D182" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E182" s="12">
         <v>916.42</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="21" t="s">
+      <c r="A183" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="B183" s="22">
+      <c r="B183" s="11">
         <v>45316</v>
       </c>
-      <c r="C183" s="21" t="s">
+      <c r="C183" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D183" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E183" s="23">
+      <c r="D183" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E183" s="12">
         <v>624.34</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="21" t="s">
+      <c r="A184" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B184" s="22">
+      <c r="B184" s="11">
         <v>45316</v>
       </c>
-      <c r="C184" s="21" t="s">
+      <c r="C184" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D184" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E184" s="23">
+      <c r="D184" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E184" s="12">
         <v>337.25</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="21" t="s">
+      <c r="A185" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B185" s="22">
+      <c r="B185" s="11">
         <v>45316</v>
       </c>
-      <c r="C185" s="21" t="s">
+      <c r="C185" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D185" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E185" s="23">
+      <c r="D185" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" s="12">
         <v>476.47</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="21" t="s">
+      <c r="A186" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="B186" s="22">
+      <c r="B186" s="11">
         <v>45316</v>
       </c>
-      <c r="C186" s="21" t="s">
+      <c r="C186" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D186" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E186" s="23">
+      <c r="D186" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E186" s="12">
         <v>193.74</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="21" t="s">
+      <c r="A187" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="B187" s="22">
+      <c r="B187" s="11">
         <v>45316</v>
       </c>
-      <c r="C187" s="21" t="s">
+      <c r="C187" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D187" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E187" s="23">
+      <c r="D187" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" s="12">
         <v>22407.17</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="21" t="s">
+      <c r="A188" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="B188" s="22">
+      <c r="B188" s="11">
         <v>45316</v>
       </c>
-      <c r="C188" s="21" t="s">
+      <c r="C188" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D188" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E188" s="23">
+      <c r="D188" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E188" s="12">
         <v>380.69</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="21" t="s">
+      <c r="A189" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="B189" s="22">
+      <c r="B189" s="11">
         <v>45316</v>
       </c>
-      <c r="C189" s="21" t="s">
+      <c r="C189" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D189" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E189" s="23">
+      <c r="D189" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E189" s="12">
         <v>2305.6999999999998</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="21" t="s">
+      <c r="A190" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="B190" s="22">
+      <c r="B190" s="11">
         <v>45316</v>
       </c>
-      <c r="C190" s="21" t="s">
+      <c r="C190" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D190" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E190" s="23">
+      <c r="D190" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E190" s="12">
         <v>274.13</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="21" t="s">
+      <c r="A191" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="B191" s="22">
+      <c r="B191" s="11">
         <v>45316</v>
       </c>
-      <c r="C191" s="21" t="s">
+      <c r="C191" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D191" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E191" s="23">
+      <c r="D191" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="12">
         <v>23736.46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
airplance chnges to checks
</commit_message>
<xml_diff>
--- a/data/raw/checks/peach tree checks.xlsx
+++ b/data/raw/checks/peach tree checks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D31AFA7-CD4A-4CCD-9486-18519F38D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C82D03-F883-4B0B-954E-226B5DAD4417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29260" yWindow="290" windowWidth="27930" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75030" yWindow="-1310" windowWidth="15350" windowHeight="19350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="278">
   <si>
     <t>Check #</t>
   </si>
@@ -819,6 +819,60 @@
   </si>
   <si>
     <t>12751</t>
+  </si>
+  <si>
+    <t>12752</t>
+  </si>
+  <si>
+    <t>12753</t>
+  </si>
+  <si>
+    <t>12754</t>
+  </si>
+  <si>
+    <t>12755</t>
+  </si>
+  <si>
+    <t>12756</t>
+  </si>
+  <si>
+    <t>12757</t>
+  </si>
+  <si>
+    <t>12758</t>
+  </si>
+  <si>
+    <t>12759</t>
+  </si>
+  <si>
+    <t>12760</t>
+  </si>
+  <si>
+    <t>James T Warring Sons Inc</t>
+  </si>
+  <si>
+    <t>12761</t>
+  </si>
+  <si>
+    <t>Alan Kinlaw</t>
+  </si>
+  <si>
+    <t>12762</t>
+  </si>
+  <si>
+    <t>12763</t>
+  </si>
+  <si>
+    <t>12764</t>
+  </si>
+  <si>
+    <t>12765</t>
+  </si>
+  <si>
+    <t>12766</t>
+  </si>
+  <si>
+    <t>12767</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1042,6 +1096,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1324,24 +1387,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K182" sqref="K182"/>
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H193" sqref="H193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="12.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +1421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1375,7 +1438,7 @@
         <v>-15000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1455,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1409,7 +1472,7 @@
         <v>82791.91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1489,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1443,7 +1506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1460,7 +1523,7 @@
         <v>926.71</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1540,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1557,7 @@
         <v>52.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1511,7 +1574,7 @@
         <v>2153.9899999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1528,7 +1591,7 @@
         <v>1916.07</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1545,7 +1608,7 @@
         <v>595.66999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1562,7 +1625,7 @@
         <v>217.56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +1642,7 @@
         <v>4744.8100000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1596,7 +1659,7 @@
         <v>373.7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1613,7 +1676,7 @@
         <v>73.98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1630,7 +1693,7 @@
         <v>306.02</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1647,7 +1710,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -1664,7 +1727,7 @@
         <v>213.22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -1681,7 +1744,7 @@
         <v>20747.71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1698,7 +1761,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1715,7 +1778,7 @@
         <v>528.08000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1795,7 @@
         <v>17055.62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -1749,7 +1812,7 @@
         <v>68633.84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
@@ -1766,7 +1829,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1783,7 +1846,7 @@
         <v>660.1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1800,7 +1863,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1817,7 +1880,7 @@
         <v>1936.51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1834,7 +1897,7 @@
         <v>3578.71</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1851,7 +1914,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -1868,7 +1931,7 @@
         <v>121.68</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -1885,7 +1948,7 @@
         <v>8272.84</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1902,7 +1965,7 @@
         <v>1489.04</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -1919,7 +1982,7 @@
         <v>42395.8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -1936,7 +1999,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -1953,7 +2016,7 @@
         <v>1802.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -1970,7 +2033,7 @@
         <v>20607.53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>76</v>
       </c>
@@ -1987,7 +2050,7 @@
         <v>25329.81</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>78</v>
       </c>
@@ -2004,7 +2067,7 @@
         <v>1038.95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="24" t="s">
         <v>79</v>
       </c>
@@ -2021,7 +2084,7 @@
         <v>564.07000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
@@ -2038,7 +2101,7 @@
         <v>920.44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="24" t="s">
         <v>82</v>
       </c>
@@ -2055,7 +2118,7 @@
         <v>104.98</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
         <v>84</v>
       </c>
@@ -2072,7 +2135,7 @@
         <v>4637.6499999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2089,7 +2152,7 @@
         <v>3226.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="24" t="s">
         <v>88</v>
       </c>
@@ -2106,7 +2169,7 @@
         <v>12709.41</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
@@ -2123,7 +2186,7 @@
         <v>340.88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
         <v>90</v>
       </c>
@@ -2140,7 +2203,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
@@ -2157,7 +2220,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>93</v>
       </c>
@@ -2174,7 +2237,7 @@
         <v>264.04000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>94</v>
       </c>
@@ -2191,7 +2254,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -2208,7 +2271,7 @@
         <v>17604.080000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -2225,7 +2288,7 @@
         <v>10086.049999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>98</v>
       </c>
@@ -2242,7 +2305,7 @@
         <v>31173.7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>100</v>
       </c>
@@ -2259,7 +2322,7 @@
         <v>3612.45</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
@@ -2276,7 +2339,7 @@
         <v>27.42</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>102</v>
       </c>
@@ -2293,7 +2356,7 @@
         <v>152.63999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
@@ -2310,7 +2373,7 @@
         <v>2862.28</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -2327,7 +2390,7 @@
         <v>104682.7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>105</v>
       </c>
@@ -2344,7 +2407,7 @@
         <v>348.75</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>106</v>
       </c>
@@ -2361,7 +2424,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>107</v>
       </c>
@@ -2378,7 +2441,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>109</v>
       </c>
@@ -2395,7 +2458,7 @@
         <v>10737.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
@@ -2412,7 +2475,7 @@
         <v>4610.13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>112</v>
       </c>
@@ -2429,7 +2492,7 @@
         <v>2049.7199999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>113</v>
       </c>
@@ -2446,7 +2509,7 @@
         <v>313.01</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>114</v>
       </c>
@@ -2463,7 +2526,7 @@
         <v>241.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>115</v>
       </c>
@@ -2480,7 +2543,7 @@
         <v>78718.11</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
@@ -2497,7 +2560,7 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>117</v>
       </c>
@@ -2514,7 +2577,7 @@
         <v>-95000</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>118</v>
       </c>
@@ -2531,7 +2594,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>119</v>
       </c>
@@ -2548,7 +2611,7 @@
         <v>2868.22</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>120</v>
       </c>
@@ -2565,7 +2628,7 @@
         <v>5262</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="21" t="s">
         <v>121</v>
       </c>
@@ -2582,7 +2645,7 @@
         <v>-1038.95</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="21" t="s">
         <v>122</v>
       </c>
@@ -2599,7 +2662,7 @@
         <v>-564.07000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="21" t="s">
         <v>123</v>
       </c>
@@ -2616,7 +2679,7 @@
         <v>-920.44</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="21" t="s">
         <v>124</v>
       </c>
@@ -2633,7 +2696,7 @@
         <v>-104.98</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="21" t="s">
         <v>125</v>
       </c>
@@ -2650,7 +2713,7 @@
         <v>-4637.6499999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="21" t="s">
         <v>126</v>
       </c>
@@ -2667,7 +2730,7 @@
         <v>-12709.41</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="21" t="s">
         <v>127</v>
       </c>
@@ -2684,7 +2747,7 @@
         <v>-2100</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
         <v>128</v>
       </c>
@@ -2701,7 +2764,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="27" t="s">
         <v>129</v>
       </c>
@@ -2718,7 +2781,7 @@
         <v>1038.95</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="27" t="s">
         <v>130</v>
       </c>
@@ -2735,7 +2798,7 @@
         <v>564.07000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="27" t="s">
         <v>131</v>
       </c>
@@ -2752,7 +2815,7 @@
         <v>1417.05</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="27" t="s">
         <v>132</v>
       </c>
@@ -2769,7 +2832,7 @@
         <v>104.98</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="27" t="s">
         <v>133</v>
       </c>
@@ -2786,7 +2849,7 @@
         <v>4637.6499999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="27" t="s">
         <v>134</v>
       </c>
@@ -2803,7 +2866,7 @@
         <v>12709.41</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>135</v>
       </c>
@@ -2820,7 +2883,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>136</v>
       </c>
@@ -2837,7 +2900,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>137</v>
       </c>
@@ -2854,7 +2917,7 @@
         <v>382.28</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>139</v>
       </c>
@@ -2871,7 +2934,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>140</v>
       </c>
@@ -2888,7 +2951,7 @@
         <v>163.24</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>142</v>
       </c>
@@ -2905,7 +2968,7 @@
         <v>855.27</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>143</v>
       </c>
@@ -2922,7 +2985,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>144</v>
       </c>
@@ -2939,7 +3002,7 @@
         <v>1870.27</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>145</v>
       </c>
@@ -2956,7 +3019,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>146</v>
       </c>
@@ -2973,7 +3036,7 @@
         <v>438.7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>147</v>
       </c>
@@ -2990,7 +3053,7 @@
         <v>329.8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -3007,7 +3070,7 @@
         <v>382.28</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -3024,7 +3087,7 @@
         <v>1824.54</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>152</v>
       </c>
@@ -3041,7 +3104,7 @@
         <v>3372.74</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>153</v>
       </c>
@@ -3058,7 +3121,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>155</v>
       </c>
@@ -3075,7 +3138,7 @@
         <v>528.08000000000004</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>156</v>
       </c>
@@ -3092,7 +3155,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>158</v>
       </c>
@@ -3109,7 +3172,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>159</v>
       </c>
@@ -3126,7 +3189,7 @@
         <v>771.38</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
@@ -3143,7 +3206,7 @@
         <v>255.26</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>162</v>
       </c>
@@ -3160,7 +3223,7 @@
         <v>91.86</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>164</v>
       </c>
@@ -3177,7 +3240,7 @@
         <v>7936.75</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>165</v>
       </c>
@@ -3194,7 +3257,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>166</v>
       </c>
@@ -3211,7 +3274,7 @@
         <v>12250</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>167</v>
       </c>
@@ -3228,7 +3291,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>169</v>
       </c>
@@ -3245,7 +3308,7 @@
         <v>1742.27</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>170</v>
       </c>
@@ -3262,7 +3325,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>171</v>
       </c>
@@ -3279,7 +3342,7 @@
         <v>2930.94</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>172</v>
       </c>
@@ -3296,7 +3359,7 @@
         <v>326.52</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>173</v>
       </c>
@@ -3313,7 +3376,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>174</v>
       </c>
@@ -3330,7 +3393,7 @@
         <v>18635</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>176</v>
       </c>
@@ -3347,7 +3410,7 @@
         <v>319.99</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="30" t="s">
         <v>177</v>
       </c>
@@ -3364,7 +3427,7 @@
         <v>583.27</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>179</v>
       </c>
@@ -3381,7 +3444,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>180</v>
       </c>
@@ -3398,7 +3461,7 @@
         <v>100.24</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>181</v>
       </c>
@@ -3415,7 +3478,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>182</v>
       </c>
@@ -3432,7 +3495,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>183</v>
       </c>
@@ -3449,7 +3512,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>185</v>
       </c>
@@ -3466,7 +3529,7 @@
         <v>84466.37</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>186</v>
       </c>
@@ -3483,7 +3546,7 @@
         <v>31594.9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>187</v>
       </c>
@@ -3497,7 +3560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>189</v>
       </c>
@@ -3511,7 +3574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
@@ -3528,7 +3591,7 @@
         <v>660.1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -3545,7 +3608,7 @@
         <v>17604.080000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>192</v>
       </c>
@@ -3562,7 +3625,7 @@
         <v>356.05</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>194</v>
       </c>
@@ -3579,7 +3642,7 @@
         <v>721.67</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>196</v>
       </c>
@@ -3596,7 +3659,7 @@
         <v>26207.99</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>197</v>
       </c>
@@ -3613,7 +3676,7 @@
         <v>25992.240000000002</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>198</v>
       </c>
@@ -3630,7 +3693,7 @@
         <v>437.13</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>200</v>
       </c>
@@ -3647,7 +3710,7 @@
         <v>819.24</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>201</v>
       </c>
@@ -3664,7 +3727,7 @@
         <v>552.08000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>203</v>
       </c>
@@ -3681,7 +3744,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>204</v>
       </c>
@@ -3698,7 +3761,7 @@
         <v>2210.7800000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>205</v>
       </c>
@@ -3715,7 +3778,7 @@
         <v>1435.63</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>206</v>
       </c>
@@ -3732,7 +3795,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>207</v>
       </c>
@@ -3749,7 +3812,7 @@
         <v>128.57</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>208</v>
       </c>
@@ -3766,7 +3829,7 @@
         <v>8824.0499999999993</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>210</v>
       </c>
@@ -3783,7 +3846,7 @@
         <v>20835.36</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>211</v>
       </c>
@@ -3800,7 +3863,7 @@
         <v>451.02</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>212</v>
       </c>
@@ -3817,7 +3880,7 @@
         <v>-31594.9</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>213</v>
       </c>
@@ -3834,7 +3897,7 @@
         <v>16751.580000000002</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>214</v>
       </c>
@@ -3851,7 +3914,7 @@
         <v>14843.32</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>215</v>
       </c>
@@ -3865,7 +3928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>216</v>
       </c>
@@ -3879,7 +3942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>213</v>
       </c>
@@ -3896,7 +3959,7 @@
         <v>16751.580000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
         <v>214</v>
       </c>
@@ -3913,7 +3976,7 @@
         <v>14843.32</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>217</v>
       </c>
@@ -3930,7 +3993,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="s">
         <v>218</v>
       </c>
@@ -3947,7 +4010,7 @@
         <v>26208.49</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="18" t="s">
         <v>219</v>
       </c>
@@ -3964,7 +4027,7 @@
         <v>518.53</v>
       </c>
     </row>
-    <row r="156" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A156" s="18" t="s">
         <v>220</v>
       </c>
@@ -3981,7 +4044,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A157" s="18" t="s">
         <v>221</v>
       </c>
@@ -3998,7 +4061,7 @@
         <v>831.49</v>
       </c>
     </row>
-    <row r="158" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A158" s="9" t="s">
         <v>222</v>
       </c>
@@ -4015,7 +4078,7 @@
         <v>1805.51</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="12" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="14" t="s">
         <v>223</v>
       </c>
@@ -4032,7 +4095,7 @@
         <v>-831.49</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A160" s="16" t="s">
         <v>224</v>
       </c>
@@ -4049,7 +4112,7 @@
         <v>472.86</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>225</v>
       </c>
@@ -4066,7 +4129,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>226</v>
       </c>
@@ -4083,7 +4146,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>227</v>
       </c>
@@ -4100,7 +4163,7 @@
         <v>801.5</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="s">
         <v>229</v>
       </c>
@@ -4117,7 +4180,7 @@
         <v>317.99</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>230</v>
       </c>
@@ -4134,7 +4197,7 @@
         <v>606.59</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="s">
         <v>231</v>
       </c>
@@ -4151,7 +4214,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="10" t="s">
         <v>233</v>
       </c>
@@ -4168,7 +4231,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>234</v>
       </c>
@@ -4185,7 +4248,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>235</v>
       </c>
@@ -4202,7 +4265,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>236</v>
       </c>
@@ -4219,7 +4282,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>237</v>
       </c>
@@ -4236,7 +4299,7 @@
         <v>264.04000000000002</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="s">
         <v>238</v>
       </c>
@@ -4253,7 +4316,7 @@
         <v>11700</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="10" t="s">
         <v>240</v>
       </c>
@@ -4270,7 +4333,7 @@
         <v>501.75</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>241</v>
       </c>
@@ -4287,7 +4350,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>242</v>
       </c>
@@ -4304,7 +4367,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>243</v>
       </c>
@@ -4321,7 +4384,7 @@
         <v>2212.8200000000002</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="s">
         <v>244</v>
       </c>
@@ -4338,7 +4401,7 @@
         <v>2617.4499999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="s">
         <v>245</v>
       </c>
@@ -4353,7 +4416,7 @@
       </c>
       <c r="E178" s="12"/>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="s">
         <v>246</v>
       </c>
@@ -4370,7 +4433,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="s">
         <v>247</v>
       </c>
@@ -4387,7 +4450,7 @@
         <v>199.16</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="s">
         <v>248</v>
       </c>
@@ -4404,7 +4467,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="s">
         <v>250</v>
       </c>
@@ -4421,7 +4484,7 @@
         <v>916.42</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="10" t="s">
         <v>251</v>
       </c>
@@ -4438,7 +4501,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="s">
         <v>252</v>
       </c>
@@ -4455,7 +4518,7 @@
         <v>337.25</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="s">
         <v>253</v>
       </c>
@@ -4472,7 +4535,7 @@
         <v>476.47</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="s">
         <v>254</v>
       </c>
@@ -4489,7 +4552,7 @@
         <v>193.74</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
         <v>255</v>
       </c>
@@ -4506,7 +4569,7 @@
         <v>22407.17</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="s">
         <v>256</v>
       </c>
@@ -4523,7 +4586,7 @@
         <v>380.69</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="s">
         <v>257</v>
       </c>
@@ -4540,7 +4603,7 @@
         <v>2305.6999999999998</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="s">
         <v>258</v>
       </c>
@@ -4557,7 +4620,7 @@
         <v>274.13</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="s">
         <v>259</v>
       </c>
@@ -4572,6 +4635,278 @@
       </c>
       <c r="E191" s="12">
         <v>23736.46</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="B192" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C192" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D192" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E192" s="35">
+        <v>552.66</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B193" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C193" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D193" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E193" s="35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B194" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C194" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D194" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E194" s="35">
+        <v>58601.78</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B195" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C195" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D195" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E195" s="35">
+        <v>14432.86</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="B196" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C196" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D196" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E196" s="35">
+        <v>33108.78</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B197" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C197" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D197" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E197" s="35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B198" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C198" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D198" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E198" s="35">
+        <v>221.63</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B199" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C199" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D199" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E199" s="35">
+        <v>1693.53</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="B200" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C200" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="D200" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="35">
+        <v>5171.72</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B201" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C201" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="D201" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B202" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C202" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D202" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="35">
+        <v>678.05</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B203" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C203" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D203" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" s="35">
+        <v>356.29</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="B204" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C204" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D204" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E204" s="35">
+        <v>2610.59</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B205" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C205" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D205" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E205" s="35">
+        <v>523.95000000000005</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="B206" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C206" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D206" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" s="35">
+        <v>404.8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="B207" s="34">
+        <v>45331</v>
+      </c>
+      <c r="C207" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D207" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="35">
+        <v>1542.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stop check functionality
</commit_message>
<xml_diff>
--- a/data/raw/checks/peach tree checks.xlsx
+++ b/data/raw/checks/peach tree checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8C514C-9946-4553-AA95-87C5046D6877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB627F3F-F6EE-472A-8838-A8E6CD9FA7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36280" yWindow="2120" windowWidth="23040" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="378">
   <si>
     <t>Check #</t>
   </si>
@@ -1023,6 +1023,156 @@
   </si>
   <si>
     <t>12810</t>
+  </si>
+  <si>
+    <t>12768V</t>
+  </si>
+  <si>
+    <t>12811</t>
+  </si>
+  <si>
+    <t>Armfield Harrison &amp; Thomas</t>
+  </si>
+  <si>
+    <t>12812</t>
+  </si>
+  <si>
+    <t>Advance Scale</t>
+  </si>
+  <si>
+    <t>12813</t>
+  </si>
+  <si>
+    <t>12814</t>
+  </si>
+  <si>
+    <t>12815</t>
+  </si>
+  <si>
+    <t>12816</t>
+  </si>
+  <si>
+    <t>12817</t>
+  </si>
+  <si>
+    <t>Town Of Bedford</t>
+  </si>
+  <si>
+    <t>12818</t>
+  </si>
+  <si>
+    <t>12819</t>
+  </si>
+  <si>
+    <t>12820</t>
+  </si>
+  <si>
+    <t>12821</t>
+  </si>
+  <si>
+    <t>12822</t>
+  </si>
+  <si>
+    <t>12823</t>
+  </si>
+  <si>
+    <t>12824</t>
+  </si>
+  <si>
+    <t>12825</t>
+  </si>
+  <si>
+    <t>12826</t>
+  </si>
+  <si>
+    <t>12827</t>
+  </si>
+  <si>
+    <t>12828</t>
+  </si>
+  <si>
+    <t>12829</t>
+  </si>
+  <si>
+    <t>12830</t>
+  </si>
+  <si>
+    <t>12831</t>
+  </si>
+  <si>
+    <t>12832</t>
+  </si>
+  <si>
+    <t>12833</t>
+  </si>
+  <si>
+    <t>12834</t>
+  </si>
+  <si>
+    <t>12835</t>
+  </si>
+  <si>
+    <t>Jordan E. Tannenbaum</t>
+  </si>
+  <si>
+    <t>12836</t>
+  </si>
+  <si>
+    <t>12837</t>
+  </si>
+  <si>
+    <t>12838</t>
+  </si>
+  <si>
+    <t>12813V</t>
+  </si>
+  <si>
+    <t>12839</t>
+  </si>
+  <si>
+    <t>12840</t>
+  </si>
+  <si>
+    <t>12841</t>
+  </si>
+  <si>
+    <t>12842</t>
+  </si>
+  <si>
+    <t>12843</t>
+  </si>
+  <si>
+    <t>12844</t>
+  </si>
+  <si>
+    <t>12845</t>
+  </si>
+  <si>
+    <t>Christopher Burris</t>
+  </si>
+  <si>
+    <t>12846</t>
+  </si>
+  <si>
+    <t>Antonio Chevalier</t>
+  </si>
+  <si>
+    <t>12847</t>
+  </si>
+  <si>
+    <t>12848</t>
+  </si>
+  <si>
+    <t>12849</t>
+  </si>
+  <si>
+    <t>Horace Foxall</t>
+  </si>
+  <si>
+    <t>12850</t>
+  </si>
+  <si>
+    <t>12851</t>
   </si>
 </sst>
 </file>
@@ -1086,9 +1236,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1096,13 +1262,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1385,24 +1544,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E294"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H230" sqref="H230"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I292" sqref="I292"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="11.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="12.61328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.61328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.61328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.69140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1436,7 +1595,7 @@
         <v>-15000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1453,7 +1612,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1470,7 +1629,7 @@
         <v>82791.91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1487,7 +1646,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +1663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1521,7 +1680,7 @@
         <v>926.71</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1538,7 +1697,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1555,7 +1714,7 @@
         <v>52.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1572,7 +1731,7 @@
         <v>2153.9899999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1589,7 +1748,7 @@
         <v>1916.07</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1606,7 +1765,7 @@
         <v>595.66999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1623,7 +1782,7 @@
         <v>217.56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1640,7 +1799,7 @@
         <v>4744.8100000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1657,7 +1816,7 @@
         <v>373.7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1674,7 +1833,7 @@
         <v>73.98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1850,7 @@
         <v>306.02</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1708,7 +1867,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -1725,7 +1884,7 @@
         <v>213.22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -1742,7 +1901,7 @@
         <v>20747.71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1759,7 +1918,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1776,7 +1935,7 @@
         <v>528.08000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1793,7 +1952,7 @@
         <v>17055.62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -1810,7 +1969,7 @@
         <v>68633.84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
@@ -1827,7 +1986,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1844,7 +2003,7 @@
         <v>660.1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1861,7 +2020,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1878,7 +2037,7 @@
         <v>1936.51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1895,7 +2054,7 @@
         <v>3578.71</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1912,7 +2071,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -1929,7 +2088,7 @@
         <v>121.68</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -1946,7 +2105,7 @@
         <v>8272.84</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1963,7 +2122,7 @@
         <v>1489.04</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -1980,7 +2139,7 @@
         <v>42395.8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -1997,7 +2156,7 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -2014,7 +2173,7 @@
         <v>1802.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -2031,7 +2190,7 @@
         <v>20607.53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>76</v>
       </c>
@@ -2048,7 +2207,7 @@
         <v>25329.81</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>78</v>
       </c>
@@ -2065,7 +2224,7 @@
         <v>1038.95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>79</v>
       </c>
@@ -2082,7 +2241,7 @@
         <v>564.07000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
@@ -2099,7 +2258,7 @@
         <v>920.44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2116,7 +2275,7 @@
         <v>104.98</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2133,7 +2292,7 @@
         <v>4637.6499999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2150,7 +2309,7 @@
         <v>3226.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2167,7 +2326,7 @@
         <v>12709.41</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
@@ -2184,7 +2343,7 @@
         <v>340.88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
@@ -2201,7 +2360,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
@@ -2218,7 +2377,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>93</v>
       </c>
@@ -2235,7 +2394,7 @@
         <v>264.04000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>94</v>
       </c>
@@ -2252,7 +2411,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -2269,7 +2428,7 @@
         <v>17604.080000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -2286,7 +2445,7 @@
         <v>10086.049999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>98</v>
       </c>
@@ -2303,7 +2462,7 @@
         <v>31173.7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>100</v>
       </c>
@@ -2320,7 +2479,7 @@
         <v>3612.45</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
@@ -2337,7 +2496,7 @@
         <v>27.42</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>102</v>
       </c>
@@ -2354,7 +2513,7 @@
         <v>152.63999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
@@ -2371,7 +2530,7 @@
         <v>2862.28</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -2388,7 +2547,7 @@
         <v>104682.7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>105</v>
       </c>
@@ -2405,7 +2564,7 @@
         <v>348.75</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>106</v>
       </c>
@@ -2422,7 +2581,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>107</v>
       </c>
@@ -2439,7 +2598,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>109</v>
       </c>
@@ -2456,7 +2615,7 @@
         <v>10737.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
@@ -2473,7 +2632,7 @@
         <v>4610.13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>112</v>
       </c>
@@ -2490,7 +2649,7 @@
         <v>2049.7199999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>113</v>
       </c>
@@ -2507,7 +2666,7 @@
         <v>313.01</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>114</v>
       </c>
@@ -2524,7 +2683,7 @@
         <v>241.5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>115</v>
       </c>
@@ -2541,7 +2700,7 @@
         <v>78718.11</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
@@ -2558,7 +2717,7 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>117</v>
       </c>
@@ -2575,7 +2734,7 @@
         <v>-95000</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>118</v>
       </c>
@@ -2592,7 +2751,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>121</v>
       </c>
@@ -2609,7 +2768,7 @@
         <v>-1038.95</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>122</v>
       </c>
@@ -2626,7 +2785,7 @@
         <v>-564.07000000000005</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>123</v>
       </c>
@@ -2643,7 +2802,7 @@
         <v>-920.44</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>124</v>
       </c>
@@ -2660,7 +2819,7 @@
         <v>-104.98</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>125</v>
       </c>
@@ -2677,7 +2836,7 @@
         <v>-4637.6499999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>126</v>
       </c>
@@ -2694,7 +2853,7 @@
         <v>-12709.41</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>127</v>
       </c>
@@ -2711,7 +2870,7 @@
         <v>-2100</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>128</v>
       </c>
@@ -2728,7 +2887,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>129</v>
       </c>
@@ -2745,7 +2904,7 @@
         <v>1038.95</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>130</v>
       </c>
@@ -2762,7 +2921,7 @@
         <v>564.07000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>131</v>
       </c>
@@ -2779,7 +2938,7 @@
         <v>1417.05</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>132</v>
       </c>
@@ -2796,7 +2955,7 @@
         <v>104.98</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>133</v>
       </c>
@@ -2813,7 +2972,7 @@
         <v>4637.6499999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>134</v>
       </c>
@@ -2830,7 +2989,7 @@
         <v>12709.41</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>120</v>
       </c>
@@ -2847,7 +3006,7 @@
         <v>5262</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>119</v>
       </c>
@@ -2864,7 +3023,7 @@
         <v>2868.22</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>135</v>
       </c>
@@ -2881,7 +3040,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>136</v>
       </c>
@@ -2898,7 +3057,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>137</v>
       </c>
@@ -2915,7 +3074,7 @@
         <v>382.28</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>139</v>
       </c>
@@ -2932,7 +3091,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>140</v>
       </c>
@@ -2949,7 +3108,7 @@
         <v>163.24</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>142</v>
       </c>
@@ -2966,7 +3125,7 @@
         <v>855.27</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>143</v>
       </c>
@@ -2983,7 +3142,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>144</v>
       </c>
@@ -3000,7 +3159,7 @@
         <v>1870.27</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>145</v>
       </c>
@@ -3017,7 +3176,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>146</v>
       </c>
@@ -3034,7 +3193,7 @@
         <v>438.7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>147</v>
       </c>
@@ -3051,7 +3210,7 @@
         <v>329.8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -3068,7 +3227,7 @@
         <v>382.28</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -3085,7 +3244,7 @@
         <v>1824.54</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>152</v>
       </c>
@@ -3102,7 +3261,7 @@
         <v>3372.74</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>153</v>
       </c>
@@ -3119,7 +3278,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>155</v>
       </c>
@@ -3136,7 +3295,7 @@
         <v>528.08000000000004</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>156</v>
       </c>
@@ -3153,7 +3312,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>158</v>
       </c>
@@ -3170,7 +3329,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>159</v>
       </c>
@@ -3187,7 +3346,7 @@
         <v>771.38</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
@@ -3204,7 +3363,7 @@
         <v>255.26</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>162</v>
       </c>
@@ -3221,7 +3380,7 @@
         <v>91.86</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>164</v>
       </c>
@@ -3238,7 +3397,7 @@
         <v>7936.75</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>165</v>
       </c>
@@ -3255,7 +3414,7 @@
         <v>454.35</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>166</v>
       </c>
@@ -3272,7 +3431,7 @@
         <v>12250</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>167</v>
       </c>
@@ -3289,7 +3448,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>169</v>
       </c>
@@ -3306,7 +3465,7 @@
         <v>1742.27</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>170</v>
       </c>
@@ -3323,7 +3482,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>171</v>
       </c>
@@ -3340,7 +3499,7 @@
         <v>2930.94</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>172</v>
       </c>
@@ -3357,7 +3516,7 @@
         <v>326.52</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>173</v>
       </c>
@@ -3374,7 +3533,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>174</v>
       </c>
@@ -3391,7 +3550,7 @@
         <v>18635</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>176</v>
       </c>
@@ -3408,7 +3567,7 @@
         <v>319.99</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>177</v>
       </c>
@@ -3425,7 +3584,7 @@
         <v>583.27</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>179</v>
       </c>
@@ -3442,7 +3601,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>180</v>
       </c>
@@ -3459,7 +3618,7 @@
         <v>100.24</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>181</v>
       </c>
@@ -3476,7 +3635,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>182</v>
       </c>
@@ -3493,7 +3652,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>183</v>
       </c>
@@ -3510,7 +3669,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>185</v>
       </c>
@@ -3527,7 +3686,7 @@
         <v>84466.37</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>186</v>
       </c>
@@ -3544,7 +3703,7 @@
         <v>31594.9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>187</v>
       </c>
@@ -3558,7 +3717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>189</v>
       </c>
@@ -3572,7 +3731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
@@ -3589,7 +3748,7 @@
         <v>660.1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -3606,7 +3765,7 @@
         <v>17604.080000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>192</v>
       </c>
@@ -3623,7 +3782,7 @@
         <v>356.05</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>194</v>
       </c>
@@ -3640,7 +3799,7 @@
         <v>721.67</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>196</v>
       </c>
@@ -3657,7 +3816,7 @@
         <v>26207.99</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>197</v>
       </c>
@@ -3674,7 +3833,7 @@
         <v>25992.240000000002</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>198</v>
       </c>
@@ -3691,7 +3850,7 @@
         <v>437.13</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>200</v>
       </c>
@@ -3708,7 +3867,7 @@
         <v>819.24</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>201</v>
       </c>
@@ -3725,7 +3884,7 @@
         <v>552.08000000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>203</v>
       </c>
@@ -3742,7 +3901,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>204</v>
       </c>
@@ -3759,7 +3918,7 @@
         <v>2210.7800000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>205</v>
       </c>
@@ -3776,7 +3935,7 @@
         <v>1435.63</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>206</v>
       </c>
@@ -3793,7 +3952,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>207</v>
       </c>
@@ -3810,7 +3969,7 @@
         <v>128.57</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>208</v>
       </c>
@@ -3827,7 +3986,7 @@
         <v>8824.0499999999993</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>210</v>
       </c>
@@ -3844,7 +4003,7 @@
         <v>20835.36</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>211</v>
       </c>
@@ -3861,7 +4020,7 @@
         <v>451.02</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>212</v>
       </c>
@@ -3878,7 +4037,7 @@
         <v>-31594.9</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>213</v>
       </c>
@@ -3895,7 +4054,7 @@
         <v>16751.580000000002</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>214</v>
       </c>
@@ -3912,7 +4071,7 @@
         <v>14843.32</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>215</v>
       </c>
@@ -3929,7 +4088,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>216</v>
       </c>
@@ -3946,7 +4105,7 @@
         <v>26208.49</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>217</v>
       </c>
@@ -3963,7 +4122,7 @@
         <v>518.53</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>218</v>
       </c>
@@ -3980,7 +4139,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>219</v>
       </c>
@@ -3997,7 +4156,7 @@
         <v>831.49</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>220</v>
       </c>
@@ -4014,7 +4173,7 @@
         <v>1805.51</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>221</v>
       </c>
@@ -4031,7 +4190,7 @@
         <v>-831.49</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>227</v>
       </c>
@@ -4048,7 +4207,7 @@
         <v>317.99</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>222</v>
       </c>
@@ -4065,7 +4224,7 @@
         <v>472.86</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>223</v>
       </c>
@@ -4082,7 +4241,7 @@
         <v>1816.3</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>224</v>
       </c>
@@ -4099,7 +4258,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>225</v>
       </c>
@@ -4116,7 +4275,7 @@
         <v>801.5</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>228</v>
       </c>
@@ -4133,7 +4292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>230</v>
       </c>
@@ -4150,7 +4309,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>231</v>
       </c>
@@ -4167,7 +4326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>232</v>
       </c>
@@ -4184,7 +4343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>324</v>
       </c>
@@ -4201,7 +4360,7 @@
         <v>29503.33</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>325</v>
       </c>
@@ -4218,7 +4377,7 @@
         <v>1705.9</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>233</v>
       </c>
@@ -4235,7 +4394,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>234</v>
       </c>
@@ -4252,7 +4411,7 @@
         <v>264.04000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>235</v>
       </c>
@@ -4269,7 +4428,7 @@
         <v>11700</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>237</v>
       </c>
@@ -4286,7 +4445,7 @@
         <v>501.75</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>238</v>
       </c>
@@ -4303,7 +4462,7 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>239</v>
       </c>
@@ -4320,7 +4479,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>240</v>
       </c>
@@ -4337,7 +4496,7 @@
         <v>2212.8200000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>241</v>
       </c>
@@ -4354,7 +4513,7 @@
         <v>2617.4499999999998</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>242</v>
       </c>
@@ -4368,7 +4527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>243</v>
       </c>
@@ -4385,7 +4544,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>244</v>
       </c>
@@ -4402,7 +4561,7 @@
         <v>199.16</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>245</v>
       </c>
@@ -4419,7 +4578,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>247</v>
       </c>
@@ -4436,7 +4595,7 @@
         <v>916.42</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>248</v>
       </c>
@@ -4453,7 +4612,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>249</v>
       </c>
@@ -4470,7 +4629,7 @@
         <v>337.25</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>250</v>
       </c>
@@ -4487,7 +4646,7 @@
         <v>476.47</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>251</v>
       </c>
@@ -4504,7 +4663,7 @@
         <v>193.74</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>252</v>
       </c>
@@ -4521,7 +4680,7 @@
         <v>22407.17</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>253</v>
       </c>
@@ -4538,7 +4697,7 @@
         <v>380.69</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>254</v>
       </c>
@@ -4555,7 +4714,7 @@
         <v>2305.6999999999998</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>255</v>
       </c>
@@ -4572,7 +4731,7 @@
         <v>274.13</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>256</v>
       </c>
@@ -4589,7 +4748,7 @@
         <v>23736.46</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>257</v>
       </c>
@@ -4606,7 +4765,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>258</v>
       </c>
@@ -4623,7 +4782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>259</v>
       </c>
@@ -4640,7 +4799,7 @@
         <v>58601.78</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>260</v>
       </c>
@@ -4657,7 +4816,7 @@
         <v>14432.86</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>261</v>
       </c>
@@ -4674,7 +4833,7 @@
         <v>33108.78</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>262</v>
       </c>
@@ -4691,7 +4850,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>263</v>
       </c>
@@ -4708,7 +4867,7 @@
         <v>221.63</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>264</v>
       </c>
@@ -4725,7 +4884,7 @@
         <v>1693.53</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>265</v>
       </c>
@@ -4742,7 +4901,7 @@
         <v>5171.72</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>267</v>
       </c>
@@ -4759,7 +4918,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>269</v>
       </c>
@@ -4776,7 +4935,7 @@
         <v>678.05</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>270</v>
       </c>
@@ -4793,7 +4952,7 @@
         <v>356.29</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>271</v>
       </c>
@@ -4810,7 +4969,7 @@
         <v>2610.59</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>272</v>
       </c>
@@ -4827,7 +4986,7 @@
         <v>523.95000000000005</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>273</v>
       </c>
@@ -4844,7 +5003,7 @@
         <v>404.8</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>274</v>
       </c>
@@ -4861,7 +5020,7 @@
         <v>1542.79</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>313</v>
       </c>
@@ -4878,7 +5037,7 @@
         <v>1735.67</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>313</v>
       </c>
@@ -4895,7 +5054,7 @@
         <v>10548.49</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>275</v>
       </c>
@@ -4912,7 +5071,7 @@
         <v>6845.3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>276</v>
       </c>
@@ -4929,7 +5088,7 @@
         <v>64118</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>277</v>
       </c>
@@ -4946,7 +5105,7 @@
         <v>17843.84</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>278</v>
       </c>
@@ -4960,7 +5119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>279</v>
       </c>
@@ -4974,7 +5133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>280</v>
       </c>
@@ -4991,7 +5150,7 @@
         <v>387.06</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>281</v>
       </c>
@@ -5008,7 +5167,7 @@
         <v>23400</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>282</v>
       </c>
@@ -5025,7 +5184,7 @@
         <v>21334.54</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>283</v>
       </c>
@@ -5042,7 +5201,7 @@
         <v>11188.5</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>285</v>
       </c>
@@ -5059,7 +5218,7 @@
         <v>25198.89</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>286</v>
       </c>
@@ -5076,7 +5235,7 @@
         <v>501.75</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>287</v>
       </c>
@@ -5093,7 +5252,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>288</v>
       </c>
@@ -5110,7 +5269,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>290</v>
       </c>
@@ -5127,7 +5286,7 @@
         <v>3455.6</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>291</v>
       </c>
@@ -5141,7 +5300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>292</v>
       </c>
@@ -5158,7 +5317,7 @@
         <v>235.34</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>293</v>
       </c>
@@ -5175,7 +5334,7 @@
         <v>2082.9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>294</v>
       </c>
@@ -5192,7 +5351,7 @@
         <v>5281.85</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>295</v>
       </c>
@@ -5209,7 +5368,7 @@
         <v>1467.41</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>296</v>
       </c>
@@ -5226,7 +5385,7 @@
         <v>337.25</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>297</v>
       </c>
@@ -5243,7 +5402,7 @@
         <v>983.09</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>298</v>
       </c>
@@ -5260,7 +5419,7 @@
         <v>137.80000000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>299</v>
       </c>
@@ -5277,7 +5436,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>301</v>
       </c>
@@ -5294,7 +5453,7 @@
         <v>1388.39</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>302</v>
       </c>
@@ -5311,7 +5470,7 @@
         <v>7392.98</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>303</v>
       </c>
@@ -5328,7 +5487,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>305</v>
       </c>
@@ -5345,7 +5504,7 @@
         <v>880.59</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>306</v>
       </c>
@@ -5362,7 +5521,7 @@
         <v>1449.57</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>307</v>
       </c>
@@ -5379,7 +5538,7 @@
         <v>2794.15</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>308</v>
       </c>
@@ -5396,7 +5555,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>309</v>
       </c>
@@ -5413,7 +5572,7 @@
         <v>43.95</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>310</v>
       </c>
@@ -5430,7 +5589,7 @@
         <v>1636.64</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>311</v>
       </c>
@@ -5447,7 +5606,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>312</v>
       </c>
@@ -5464,7 +5623,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>314</v>
       </c>
@@ -5481,7 +5640,7 @@
         <v>-235.34</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>315</v>
       </c>
@@ -5498,7 +5657,7 @@
         <v>-17843.84</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>316</v>
       </c>
@@ -5515,7 +5674,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>317</v>
       </c>
@@ -5532,7 +5691,7 @@
         <v>9662.34</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>318</v>
       </c>
@@ -5549,7 +5708,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>319</v>
       </c>
@@ -5566,7 +5725,7 @@
         <v>117.67</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>320</v>
       </c>
@@ -5583,7 +5742,7 @@
         <v>624.34</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>321</v>
       </c>
@@ -5600,7 +5759,7 @@
         <v>524.91</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>323</v>
       </c>
@@ -5617,7 +5776,7 @@
         <v>355.5</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>326</v>
       </c>
@@ -5634,7 +5793,7 @@
         <v>552.66</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>327</v>
       </c>
@@ -5649,6 +5808,731 @@
       </c>
       <c r="E251" s="4">
         <v>406.87</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A252" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B252" s="3">
+        <v>45362</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E252" s="4">
+        <v>-6845.3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A253" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B253" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E253" s="4">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A254" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B254" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E254" s="4">
+        <v>6845.3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A255" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B255" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E255" s="4">
+        <v>17843.84</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A256" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B256" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A257" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B257" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A258" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B258" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E258" s="4">
+        <v>660.1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A259" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B259" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E259" s="4">
+        <v>82.86</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A260" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B260" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E260" s="4">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A261" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B261" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E261" s="4">
+        <v>20484.02</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A262" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B262" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E262" s="4">
+        <v>16938.73</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A263" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B263" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E263" s="4">
+        <v>535.97</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A264" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B264" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E264" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A265" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B265" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E265" s="4">
+        <v>3089.9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A266" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B266" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E266" s="4">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A267" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B267" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E267" s="4">
+        <v>199.81</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A268" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B268" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E268" s="4">
+        <v>1637.65</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A269" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B269" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E269" s="4">
+        <v>3769.71</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A270" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B270" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E270" s="4">
+        <v>1248.68</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A271" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B271" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E271" s="4">
+        <v>968.85</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A272" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B272" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E272" s="4">
+        <v>6904</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A273" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B273" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E273" s="4">
+        <v>137.80000000000001</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A274" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B274" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E274" s="4">
+        <v>23721.17</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A275" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B275" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E275" s="4">
+        <v>9477.27</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A276" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B276" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E276" s="4">
+        <v>50.88</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A277" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B277" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E277" s="4">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A278" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B278" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E278" s="4">
+        <v>12762.63</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A279" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B279" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E279" s="4">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A280" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B280" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D280" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E280" s="4">
+        <v>1651.63</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A281" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B281" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E281" s="4">
+        <v>-17843.84</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A282" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B282" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D282" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E282" s="4">
+        <v>264.04000000000002</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A283" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B283" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D283" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E283" s="4">
+        <v>251.21</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A284" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B284" s="3">
+        <v>45371</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D284" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E284" s="4">
+        <v>751.44</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A285" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B285" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C285" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D285" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E285" s="10">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A286" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B286" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C286" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D286" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E286" s="10">
+        <v>552.66</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A287" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B287" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C287" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D287" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E287" s="10">
+        <v>26741.38</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A288" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B288" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C288" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D288" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E288" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A289" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B289" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C289" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D289" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E289" s="10">
+        <v>138.4</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A290" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="B290" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C290" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D290" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E290" s="10">
+        <v>30128.36</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A291" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B291" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C291" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D291" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E291" s="10">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A292" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B292" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C292" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="D292" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E292" s="10">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A293" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B293" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C293" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D293" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E293" s="10">
+        <v>400.31</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A294" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B294" s="9">
+        <v>45390</v>
+      </c>
+      <c r="C294" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D294" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E294" s="10">
+        <v>215.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checks processed 13 may
</commit_message>
<xml_diff>
--- a/data/raw/checks/peach tree checks.xlsx
+++ b/data/raw/checks/peach tree checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F705FBEC-A342-4918-AC07-691290C79FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AACC03-4E18-4268-8173-201CF3DAECC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36190" yWindow="1920" windowWidth="21130" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30890" yWindow="430" windowWidth="26770" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="434">
   <si>
     <t>Check #</t>
   </si>
@@ -1263,6 +1263,84 @@
   </si>
   <si>
     <t>12876</t>
+  </si>
+  <si>
+    <t>12377</t>
+  </si>
+  <si>
+    <t>on line paid 4/30/24</t>
+  </si>
+  <si>
+    <t>12878</t>
+  </si>
+  <si>
+    <t>12879</t>
+  </si>
+  <si>
+    <t>12880</t>
+  </si>
+  <si>
+    <t>12881</t>
+  </si>
+  <si>
+    <t>Alpha Analytical, Inc</t>
+  </si>
+  <si>
+    <t>12882</t>
+  </si>
+  <si>
+    <t>12883</t>
+  </si>
+  <si>
+    <t>12884</t>
+  </si>
+  <si>
+    <t>12885</t>
+  </si>
+  <si>
+    <t>CohnReznick</t>
+  </si>
+  <si>
+    <t>12886</t>
+  </si>
+  <si>
+    <t>12887</t>
+  </si>
+  <si>
+    <t>ID Discovery Inc</t>
+  </si>
+  <si>
+    <t>12888</t>
+  </si>
+  <si>
+    <t>12889</t>
+  </si>
+  <si>
+    <t>Labelmaster</t>
+  </si>
+  <si>
+    <t>12890</t>
+  </si>
+  <si>
+    <t>12891</t>
+  </si>
+  <si>
+    <t>New Pig Corporation</t>
+  </si>
+  <si>
+    <t>12892</t>
+  </si>
+  <si>
+    <t>12893</t>
+  </si>
+  <si>
+    <t>12894</t>
+  </si>
+  <si>
+    <t>12895</t>
+  </si>
+  <si>
+    <t>12896</t>
   </si>
 </sst>
 </file>
@@ -1351,6 +1429,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1359,9 +1440,6 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1643,11 +1721,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E320"/>
+  <dimension ref="A1:E341"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A312" sqref="A312:A320"/>
+      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -6921,156 +6999,513 @@
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="11" t="s">
+      <c r="A312" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="B312" s="9">
+      <c r="B312" s="3">
         <v>45412</v>
       </c>
-      <c r="C312" s="8" t="s">
+      <c r="C312" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D312" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E312" s="10">
+      <c r="D312" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E312" s="4">
         <v>11000</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="11" t="s">
+      <c r="A313" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="B313" s="9">
+      <c r="B313" s="3">
         <v>45412</v>
       </c>
-      <c r="C313" s="8" t="s">
+      <c r="C313" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D313" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E313" s="10">
+      <c r="D313" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E313" s="4">
         <v>17604.080000000002</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="11" t="s">
+      <c r="A314" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="B314" s="9">
+      <c r="B314" s="3">
         <v>45412</v>
       </c>
-      <c r="C314" s="8" t="s">
+      <c r="C314" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D314" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E314" s="10">
+      <c r="D314" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E314" s="4">
         <v>3900</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="11" t="s">
+      <c r="A315" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="B315" s="9">
+      <c r="B315" s="3">
         <v>45412</v>
       </c>
-      <c r="C315" s="8" t="s">
+      <c r="C315" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D315" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E315" s="10">
+      <c r="D315" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E315" s="4">
         <v>17500</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A316" s="11" t="s">
+      <c r="A316" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="B316" s="9">
+      <c r="B316" s="3">
         <v>45412</v>
       </c>
-      <c r="C316" s="8" t="s">
+      <c r="C316" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D316" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E316" s="10">
+      <c r="D316" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E316" s="4">
         <v>19406</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="11" t="s">
+      <c r="A317" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="B317" s="9">
+      <c r="B317" s="3">
         <v>45412</v>
       </c>
-      <c r="C317" s="8" t="s">
+      <c r="C317" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D317" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E317" s="10">
+      <c r="D317" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E317" s="4">
         <v>1189.47</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="11" t="s">
+      <c r="A318" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="B318" s="9">
+      <c r="B318" s="3">
         <v>45412</v>
       </c>
-      <c r="C318" s="8" t="s">
+      <c r="C318" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D318" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E318" s="10">
+      <c r="D318" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E318" s="4">
         <v>3500</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A319" s="11" t="s">
+      <c r="A319" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="B319" s="9">
+      <c r="B319" s="3">
         <v>45412</v>
       </c>
-      <c r="C319" s="8" t="s">
+      <c r="C319" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D319" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E319" s="10">
+      <c r="D319" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E319" s="4">
         <v>94.5</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" s="11" t="s">
+      <c r="A320" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B320" s="9">
+      <c r="B320" s="3">
         <v>45412</v>
       </c>
-      <c r="C320" s="8" t="s">
+      <c r="C320" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D320" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E320" s="10">
+      <c r="D320" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E320" s="4">
         <v>547.49</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A321" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B321" s="10">
+        <v>45412</v>
+      </c>
+      <c r="C321" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D321" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E321" s="11">
+        <v>1089.0999999999999</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A322" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="B322" s="10">
+        <v>45412</v>
+      </c>
+      <c r="C322" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D322" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E322" s="11">
+        <v>1584.24</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A323" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B323" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C323" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D323" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E323" s="11">
+        <v>23335.79</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A324" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="B324" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C324" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D324" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E324" s="11">
+        <v>415115.53</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A325" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B325" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C325" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D325" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E325" s="11">
+        <v>131610.79999999999</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A326" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B326" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C326" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="D326" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E326" s="11">
+        <v>638.79999999999995</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B327" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C327" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D327" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E327" s="11">
+        <v>963.3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A328" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B328" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C328" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D328" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E328" s="11">
+        <v>12605</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A329" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="B329" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C329" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D329" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E329" s="11">
+        <v>11338.02</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A330" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B330" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C330" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D330" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E330" s="11">
+        <v>7074.37</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B331" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C331" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D331" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E331" s="11">
+        <v>1478.43</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A332" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B332" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C332" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="D332" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E332" s="11">
+        <v>10010</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A333" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="B333" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C333" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D333" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E333" s="11">
+        <v>1401.72</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A334" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B334" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C334" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D334" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E334" s="11">
+        <v>541.98</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A335" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="B335" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C335" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D335" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E335" s="11">
+        <v>624.34</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B336" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C336" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="D336" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E336" s="11">
+        <v>15139.55</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="B337" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C337" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D337" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E337" s="11">
+        <v>137.80000000000001</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A338" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="B338" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C338" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D338" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E338" s="11">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A339" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="B339" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C339" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D339" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E339" s="11">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A340" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="B340" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C340" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D340" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E340" s="11">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A341" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="B341" s="10">
+        <v>45425</v>
+      </c>
+      <c r="C341" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D341" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E341" s="11">
+        <v>339.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>